<commit_message>
All sizing functions tested and passing
</commit_message>
<xml_diff>
--- a/test/desgn_params_VV.xlsx
+++ b/test/desgn_params_VV.xlsx
@@ -1,26 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexisPC\PycharmProjects\DSE-Mars-Reveal\project\subsystems_design\AOCS\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\lmaio\Nextcloud\TU Delft\2019-2020\DSE-Mars-Reveal\project\subsystems_design\AOCS\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772D630F-8DA0-423B-9844-231603290CA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="25560" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="25560" windowHeight="13020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PRIMARY INPUTS" sheetId="6" r:id="rId1"/>
     <sheet name="hardware" sheetId="3" r:id="rId2"/>
     <sheet name="orb_mission" sheetId="1" r:id="rId3"/>
     <sheet name="orb_props" sheetId="2" r:id="rId4"/>
-    <sheet name="probe_props" sheetId="4" r:id="rId5"/>
-    <sheet name="probe_mission" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
   <si>
     <t>value</t>
   </si>
@@ -163,12 +160,6 @@
     <t>probe_mass</t>
   </si>
   <si>
-    <t>n_thrusters</t>
-  </si>
-  <si>
-    <t>cold_gas_rho</t>
-  </si>
-  <si>
     <t>app_slew</t>
   </si>
   <si>
@@ -208,16 +199,13 @@
     <t>orbiter_SA_mass</t>
   </si>
   <si>
-    <t>full orbiter slew maneuver using thrusters</t>
-  </si>
-  <si>
-    <t>kg/m3</t>
+    <t>12/yr for 5 yrs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000E+00"/>
   </numFmts>
@@ -558,10 +546,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -605,7 +593,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>25</v>
@@ -621,7 +609,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:S8"/>
   <sheetViews>
@@ -670,7 +658,7 @@
         <v>36</v>
       </c>
       <c r="K1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -743,7 +731,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -789,7 +777,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
@@ -833,7 +821,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
@@ -861,10 +849,10 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E8">
         <f>25/899</f>
@@ -878,7 +866,7 @@
         <v>7.2302558398220241E-3</v>
       </c>
       <c r="L8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q8">
         <v>1.3</v>
@@ -897,12 +885,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,7 +911,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -962,10 +950,10 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -973,7 +961,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -984,7 +972,7 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>3000</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -995,7 +983,7 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1009,12 +997,12 @@
         <v>0.05</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10">
         <v>90</v>
@@ -1023,12 +1011,12 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B11">
         <v>120</v>
@@ -1037,7 +1025,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1047,12 +1035,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,98 +1048,6 @@
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4">
-        <v>23.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8">
-        <f>'PRIMARY INPUTS'!B2</f>
-        <v>3284.166976</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
@@ -1162,56 +1058,64 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="B2">
-        <f>'PRIMARY INPUTS'!B3</f>
-        <v>211.11133659999999</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B4">
-        <v>280</v>
-      </c>
-      <c r="C4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>215</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>